<commit_message>
Modified the DeleteRecord test cases from Hardcoded to data driven from excel
</commit_message>
<xml_diff>
--- a/TestData/RegisterTestData.xlsx
+++ b/TestData/RegisterTestData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaith\eclipse-workspace\Vaitheeswaran_Sundararaj_teladoc_challenge\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaith\OneDrive\Documents\KeepMeUpdated\Teladoc\Assignment\Completed\Vaitheeswaran_Sundararaj_teladoc_challenge\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0889EB1E-44D6-4D27-81E0-22EB5F8AF1FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5808BBD1-1C88-48CA-826D-0428969FFF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-8655" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterData" sheetId="1" r:id="rId1"/>
+    <sheet name="DeleteRecord" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>FirstName</t>
   </si>
@@ -98,6 +99,9 @@
   </si>
   <si>
     <t>NameRamTeladoc@gmail.com</t>
+  </si>
+  <si>
+    <t>novak</t>
   </si>
 </sst>
 </file>
@@ -432,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,4 +538,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A290AB-0442-43D2-8F80-C6EECB6DD108}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>